<commit_message>
Updated Location Logic for EmoTracker
</commit_message>
<xml_diff>
--- a/data/LocationLogic.xlsx
+++ b/data/LocationLogic.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="256">
   <si>
     <t>Jeweler Reward 1</t>
   </si>
@@ -778,6 +778,12 @@
   </si>
   <si>
     <t>Father's Journal</t>
+  </si>
+  <si>
+    <t>Any Will Ability</t>
+  </si>
+  <si>
+    <t>ANY WILL ABILITY</t>
   </si>
 </sst>
 </file>
@@ -879,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -921,6 +927,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1224,11 +1236,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q243"/>
+  <dimension ref="A1:Q239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,11 +1297,11 @@
     </row>
     <row r="3" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>193</v>
+        <v>255</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="16" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -1300,7 +1312,7 @@
       <c r="A4" s="8"/>
       <c r="C4" s="10"/>
       <c r="D4" s="16" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -1311,18 +1323,12 @@
       <c r="A5" s="8"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="H5" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1335,7 +1341,7 @@
     </row>
     <row r="7" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
@@ -1349,12 +1355,10 @@
     <row r="8" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>201</v>
-      </c>
+      <c r="D8" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1362,15 +1366,21 @@
     <row r="9" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="18" t="s">
-        <v>202</v>
+      <c r="D9" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+        <v>190</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1383,11 +1393,11 @@
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1398,10 +1408,10 @@
       <c r="A12" s="8"/>
       <c r="C12" s="10"/>
       <c r="D12" s="18" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1411,10 +1421,10 @@
       <c r="A13" s="8"/>
       <c r="C13" s="10"/>
       <c r="D13" s="18" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1431,15 +1441,13 @@
     </row>
     <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>214</v>
-      </c>
+      <c r="D15" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1448,255 +1456,269 @@
       <c r="A16" s="8"/>
       <c r="C16" s="10"/>
       <c r="D16" s="18" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>211</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="C19" s="10"/>
       <c r="D19" s="18" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="20" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="18" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>148</v>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>216</v>
+      <c r="D33" s="12" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="D34" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>216</v>
+      <c r="A36" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>149</v>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>154</v>
@@ -1707,215 +1729,186 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>216</v>
-      </c>
+    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>216</v>
+      <c r="A43" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>183</v>
+      <c r="D44" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>183</v>
+      <c r="D45" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D46" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>185</v>
+      <c r="D46" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>185</v>
+      <c r="D47" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>235</v>
+        <v>16</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E49" s="6" t="s">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>150</v>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D52" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>21</v>
+        <v>235</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="F53" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>196</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>182</v>
-      </c>
+      <c r="G53" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>196</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>195</v>
+      <c r="A55" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>184</v>
@@ -1924,81 +1917,90 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D59" s="14" t="s">
+      <c r="C61" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>154</v>
@@ -2006,10 +2008,13 @@
       <c r="D65" s="12" t="s">
         <v>189</v>
       </c>
+      <c r="E65" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>154</v>
@@ -2017,147 +2022,171 @@
       <c r="D66" s="12" t="s">
         <v>189</v>
       </c>
+      <c r="E66" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>189</v>
       </c>
+      <c r="E67" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>189</v>
       </c>
+      <c r="E68" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>190</v>
+      <c r="E69" s="19" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>218</v>
+        <v>30</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="E70" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>191</v>
+      <c r="E70" s="19" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="F71" s="6" t="s">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>218</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G72" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="H72" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-    </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D74" s="17" t="s">
+      <c r="C76" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D76" s="17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>34</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>154</v>
@@ -2168,7 +2197,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>154</v>
@@ -2179,7 +2208,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>154</v>
@@ -2190,80 +2219,74 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="B84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>40</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>41</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>196</v>
+        <v>40</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>196</v>
+        <v>41</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>195</v>
+        <v>186</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,78 +2397,72 @@
       <c r="D96" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E96" s="6" t="s">
-        <v>194</v>
+      <c r="E96" s="19" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>196</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D98" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>195</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D99" s="17" t="s">
+      <c r="A99" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D100" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E99" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="H99" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>162</v>
+      <c r="B101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D101" s="17" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>154</v>
@@ -2456,7 +2473,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>154</v>
@@ -2464,10 +2481,13 @@
       <c r="D103" s="17" t="s">
         <v>186</v>
       </c>
+      <c r="E103" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>154</v>
@@ -2475,10 +2495,13 @@
       <c r="D104" s="17" t="s">
         <v>186</v>
       </c>
+      <c r="E104" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>154</v>
@@ -2486,13 +2509,10 @@
       <c r="D105" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E105" s="6" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>154</v>
@@ -2501,43 +2521,40 @@
         <v>186</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>196</v>
+        <v>56</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="D107" s="17" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>196</v>
+        <v>57</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="D108" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D109" s="17" t="s">
         <v>186</v>
@@ -2545,107 +2562,104 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D110" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E110" s="6" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D111" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>57</v>
+        <v>230</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
       <c r="D112" s="17" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>58</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D113" s="17" t="s">
-        <v>186</v>
-      </c>
+      <c r="E112" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D114" s="17" t="s">
-        <v>186</v>
+      <c r="A114" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D115" s="17" t="s">
-        <v>186</v>
+        <v>154</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>230</v>
+        <v>62</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D116" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
-      <c r="C117" s="7"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="7"/>
-      <c r="G117" s="7"/>
-      <c r="H117" s="7"/>
+        <v>154</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>63</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>163</v>
+      <c r="B118" t="s">
+        <v>64</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>154</v>
@@ -2653,88 +2667,91 @@
       <c r="D119" s="14" t="s">
         <v>206</v>
       </c>
+      <c r="E119" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D120" s="14" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>63</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>206</v>
-      </c>
+    <row r="121" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
+      <c r="G121" s="7"/>
+      <c r="H121" s="7"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>64</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D122" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="E122" s="6" t="s">
-        <v>204</v>
+      <c r="A122" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="3"/>
-      <c r="C125" s="7"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="7"/>
-      <c r="F125" s="7"/>
-      <c r="G125" s="7"/>
-      <c r="H125" s="7"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>69</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>164</v>
+      <c r="B126" t="s">
+        <v>70</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>154</v>
@@ -2742,10 +2759,13 @@
       <c r="D127" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E127" s="6" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>154</v>
@@ -2753,10 +2773,13 @@
       <c r="D128" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E128" s="6" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>154</v>
@@ -2764,13 +2787,16 @@
       <c r="D129" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E129" s="6" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>202</v>
@@ -2778,30 +2804,27 @@
       <c r="E130" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F130" s="6" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>202</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>72</v>
+        <v>227</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="D132" s="14" t="s">
         <v>202</v>
@@ -2809,83 +2832,77 @@
       <c r="E132" s="6" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>73</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>228</v>
-      </c>
+      <c r="F132" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+      <c r="H133" s="7"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>74</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D134" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E134" s="6" t="s">
-        <v>226</v>
+      <c r="A134" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D135" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E135" s="6" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>227</v>
+        <v>77</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="D136" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E136" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F136" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="3"/>
-      <c r="C137" s="7"/>
-      <c r="D137" s="13"/>
-      <c r="E137" s="7"/>
-      <c r="F137" s="7"/>
-      <c r="G137" s="7"/>
-      <c r="H137" s="7"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>78</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D137" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>165</v>
+      <c r="B138" t="s">
+        <v>79</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D138" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>154</v>
@@ -2893,21 +2910,27 @@
       <c r="D139" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E139" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D140" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E140" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>154</v>
@@ -2921,10 +2944,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>79</v>
+        <v>232</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="D142" s="14" t="s">
         <v>202</v>
@@ -2932,38 +2955,27 @@
       <c r="E142" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>80</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E143" s="6" t="s">
-        <v>182</v>
-      </c>
+      <c r="F142" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3"/>
+      <c r="C143" s="7"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7"/>
+      <c r="G143" s="7"/>
+      <c r="H143" s="7"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>81</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D144" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E144" s="6" t="s">
-        <v>182</v>
+      <c r="A144" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>154</v>
@@ -2971,77 +2983,68 @@
       <c r="D145" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E145" s="6" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>232</v>
+        <v>84</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="D146" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E146" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F146" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="3"/>
-      <c r="C147" s="7"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
-      <c r="H147" s="7"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>85</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D147" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>166</v>
+      <c r="B148" t="s">
+        <v>86</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D149" s="14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C150" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>202</v>
-      </c>
+    <row r="150" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="3"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7"/>
+      <c r="H150" s="7"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>85</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D151" s="14" t="s">
-        <v>202</v>
+      <c r="A151" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>154</v>
@@ -3052,35 +3055,43 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D153" s="14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="3"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="13"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-      <c r="H154" s="7"/>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>90</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D154" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>167</v>
+      <c r="B155" t="s">
+        <v>91</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D155" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D156" s="14" t="s">
         <v>202</v>
@@ -3088,10 +3099,10 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D157" s="14" t="s">
         <v>202</v>
@@ -3099,96 +3110,96 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>154</v>
+        <v>236</v>
       </c>
       <c r="D158" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E158" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="D159" s="14" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>92</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D160" s="14" t="s">
-        <v>202</v>
-      </c>
+      <c r="E159" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
+      <c r="G160" s="7"/>
+      <c r="H160" s="7"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>93</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>202</v>
+      <c r="A161" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>236</v>
+        <v>154</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>239</v>
+        <v>96</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>219</v>
+        <v>154</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E163" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="F163" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="3"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="13"/>
-      <c r="E164" s="7"/>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-      <c r="H164" s="7"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>97</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D164" s="14" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
-        <v>168</v>
+      <c r="B165" t="s">
+        <v>98</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D165" s="14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>154</v>
@@ -3199,7 +3210,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>154</v>
@@ -3210,7 +3221,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>154</v>
@@ -3218,43 +3229,38 @@
       <c r="D168" s="14" t="s">
         <v>212</v>
       </c>
+      <c r="E168" s="6" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D169" s="14" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>99</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D170" s="14" t="s">
-        <v>212</v>
-      </c>
+    <row r="170" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="3"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="7"/>
+      <c r="F170" s="7"/>
+      <c r="G170" s="7"/>
+      <c r="H170" s="7"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>100</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D171" s="14" t="s">
-        <v>212</v>
+      <c r="A171" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>154</v>
@@ -3263,37 +3269,60 @@
         <v>212</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D173" s="14" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="3"/>
-      <c r="C174" s="7"/>
-      <c r="D174" s="13"/>
-      <c r="E174" s="7"/>
-      <c r="F174" s="7"/>
-      <c r="G174" s="7"/>
-      <c r="H174" s="7"/>
+      <c r="E173" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>105</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D174" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
-        <v>169</v>
+      <c r="B175" t="s">
+        <v>106</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D175" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E175" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F175" s="6" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>154</v>
@@ -3304,13 +3333,16 @@
       <c r="E176" s="6" t="s">
         <v>195</v>
       </c>
+      <c r="F176" s="6" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D177" s="14" t="s">
         <v>212</v>
@@ -3321,10 +3353,10 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D178" s="14" t="s">
         <v>212</v>
@@ -3332,16 +3364,13 @@
       <c r="E178" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F178" s="6" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D179" s="14" t="s">
         <v>212</v>
@@ -3355,10 +3384,10 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>107</v>
+        <v>250</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>154</v>
+        <v>249</v>
       </c>
       <c r="D180" s="14" t="s">
         <v>212</v>
@@ -3369,101 +3398,78 @@
       <c r="F180" s="6" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>108</v>
-      </c>
-      <c r="C181" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D181" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E181" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="G180" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7"/>
+      <c r="G181" s="7"/>
+      <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>109</v>
-      </c>
-      <c r="C182" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D182" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E182" s="6" t="s">
-        <v>195</v>
+      <c r="A182" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D183" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E183" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="F183" s="6" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>250</v>
+        <v>112</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>249</v>
+        <v>154</v>
       </c>
       <c r="D184" s="14" t="s">
         <v>212</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="F184" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="G184" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="I184" s="6"/>
-    </row>
-    <row r="185" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="3"/>
-      <c r="C185" s="7"/>
-      <c r="D185" s="13"/>
-      <c r="E185" s="7"/>
-      <c r="F185" s="7"/>
-      <c r="G185" s="7"/>
-      <c r="H185" s="7"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>113</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D185" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="3"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="7"/>
+      <c r="F186" s="7"/>
+      <c r="G186" s="7"/>
+      <c r="H186" s="7"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
-        <v>111</v>
-      </c>
-      <c r="C187" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D187" s="14" t="s">
-        <v>212</v>
+      <c r="A187" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>154</v>
@@ -3471,38 +3477,70 @@
       <c r="D188" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E188" s="6" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D189" s="14" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="3"/>
-      <c r="C190" s="7"/>
-      <c r="D190" s="13"/>
-      <c r="E190" s="7"/>
-      <c r="F190" s="7"/>
-      <c r="G190" s="7"/>
-      <c r="H190" s="7"/>
+      <c r="E189" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F189" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>116</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D190" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G190" s="6" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>171</v>
+      <c r="B191" t="s">
+        <v>196</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D191" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G191" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H191" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>154</v>
@@ -3510,27 +3548,42 @@
       <c r="D192" s="14" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E192" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F192" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G192" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="F193" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G193" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H193" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>154</v>
@@ -3545,10 +3598,14 @@
         <v>195</v>
       </c>
       <c r="G194" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H194" s="6" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I194" s="6"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>196</v>
       </c>
@@ -3565,15 +3622,18 @@
         <v>196</v>
       </c>
       <c r="G195" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H195" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="H195" s="6" t="s">
+      <c r="I195" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>154</v>
@@ -3588,10 +3648,14 @@
         <v>195</v>
       </c>
       <c r="G196" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H196" s="6" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I196" s="6"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>196</v>
       </c>
@@ -3608,15 +3672,18 @@
         <v>196</v>
       </c>
       <c r="G197" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H197" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="H197" s="6" t="s">
+      <c r="I197" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>154</v>
@@ -3638,7 +3705,7 @@
       </c>
       <c r="I198" s="6"/>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>196</v>
       </c>
@@ -3664,12 +3731,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>212</v>
@@ -3680,46 +3747,30 @@
       <c r="F200" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G200" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H200" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="I200" s="6"/>
-    </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>196</v>
+        <v>122</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F201" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="G201" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H201" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="I201" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D202" s="14" t="s">
         <v>212</v>
@@ -3730,191 +3781,143 @@
       <c r="F202" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G202" s="6" t="s">
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>248</v>
+      </c>
+      <c r="C203" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D203" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F203" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G203" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="H202" s="6" t="s">
+      <c r="H203" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="I202" s="6"/>
-    </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
+      <c r="I203" s="6"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
         <v>196</v>
       </c>
-      <c r="C203" s="6" t="s">
+      <c r="C204" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D203" s="14" t="s">
+      <c r="D204" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E203" s="6" t="s">
+      <c r="E204" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="F203" s="6" t="s">
+      <c r="F204" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="G203" s="6" t="s">
+      <c r="G204" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="H203" s="6" t="s">
+      <c r="H204" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="I203" s="6" t="s">
+      <c r="I204" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>121</v>
-      </c>
-      <c r="C204" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D204" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E204" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F204" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
-        <v>122</v>
-      </c>
-      <c r="C205" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D205" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E205" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F205" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>123</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D206" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E206" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F206" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="13"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
+      <c r="G205" s="7"/>
+      <c r="H205" s="7"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>248</v>
+        <v>124</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>249</v>
+        <v>154</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E207" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F207" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="G207" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H207" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="I207" s="6"/>
-    </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="C208" s="6" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="D208" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E208" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F208" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="G208" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H208" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="I208" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="3"/>
-      <c r="C209" s="7"/>
-      <c r="D209" s="13"/>
-      <c r="E209" s="7"/>
-      <c r="F209" s="7"/>
-      <c r="G209" s="7"/>
-      <c r="H209" s="7"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>126</v>
+      </c>
+      <c r="C209" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D209" s="14" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>172</v>
+      <c r="B210" t="s">
+        <v>127</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D210" s="14" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C211" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D211" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>125</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D212" s="14" t="s">
-        <v>220</v>
-      </c>
+    <row r="212" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3"/>
+      <c r="C212" s="7"/>
+      <c r="D212" s="13"/>
+      <c r="E212" s="7"/>
+      <c r="F212" s="7"/>
+      <c r="G212" s="7"/>
+      <c r="H212" s="7"/>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>126</v>
-      </c>
-      <c r="C213" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D213" s="14" t="s">
-        <v>220</v>
+      <c r="A213" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>154</v>
@@ -3925,32 +3928,52 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D215" s="14" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="3"/>
-      <c r="C216" s="7"/>
-      <c r="D216" s="13"/>
-      <c r="E216" s="7"/>
-      <c r="F216" s="7"/>
-      <c r="G216" s="7"/>
-      <c r="H216" s="7"/>
+      <c r="E215" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>131</v>
+      </c>
+      <c r="C216" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D216" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E216" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F216" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
-        <v>173</v>
+      <c r="B217" t="s">
+        <v>132</v>
+      </c>
+      <c r="C217" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D217" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E217" s="6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>154</v>
@@ -3958,10 +3981,13 @@
       <c r="D218" s="14" t="s">
         <v>220</v>
       </c>
+      <c r="E218" s="6" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>154</v>
@@ -3972,10 +3998,13 @@
       <c r="E219" s="6" t="s">
         <v>224</v>
       </c>
+      <c r="F219" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>154</v>
@@ -3986,13 +4015,10 @@
       <c r="E220" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F220" s="6" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>154</v>
@@ -4003,10 +4029,13 @@
       <c r="E221" s="6" t="s">
         <v>224</v>
       </c>
+      <c r="F221" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>154</v>
@@ -4017,10 +4046,13 @@
       <c r="E222" s="6" t="s">
         <v>224</v>
       </c>
+      <c r="F222" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>154</v>
@@ -4031,13 +4063,10 @@
       <c r="E223" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F223" s="6" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>154</v>
@@ -4051,7 +4080,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>154</v>
@@ -4062,16 +4091,13 @@
       <c r="E225" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F225" s="6" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D226" s="14" t="s">
         <v>220</v>
@@ -4079,114 +4105,114 @@
       <c r="E226" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F226" s="6" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="D227" s="14" t="s">
         <v>220</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
-        <v>139</v>
-      </c>
-      <c r="C228" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D228" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="E228" s="6" t="s">
-        <v>224</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="F227" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="3"/>
+      <c r="C228" s="7"/>
+      <c r="D228" s="13"/>
+      <c r="E228" s="7"/>
+      <c r="F228" s="7"/>
+      <c r="G228" s="7"/>
+      <c r="H228" s="7"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
-        <v>140</v>
-      </c>
-      <c r="C229" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D229" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="E229" s="6" t="s">
-        <v>224</v>
+      <c r="A229" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D230" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="E230" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>251</v>
+        <v>143</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>219</v>
+        <v>154</v>
       </c>
       <c r="D231" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="F231" s="6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="3"/>
-      <c r="C232" s="7"/>
-      <c r="D232" s="13"/>
-      <c r="E232" s="7"/>
-      <c r="F232" s="7"/>
-      <c r="G232" s="7"/>
-      <c r="H232" s="7"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>144</v>
+      </c>
+      <c r="C232" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D232" s="14" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
-        <v>174</v>
+      <c r="B233" t="s">
+        <v>145</v>
+      </c>
+      <c r="C233" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D233" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E233" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F233" s="6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D234" s="14" t="s">
-        <v>221</v>
+        <v>196</v>
+      </c>
+      <c r="D234" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E234" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="D235" s="14" t="s">
         <v>221</v>
@@ -4200,93 +4226,34 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="C236" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D236" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B237" t="s">
-        <v>145</v>
-      </c>
-      <c r="C237" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D237" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="E237" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F237" s="6" t="s">
-        <v>224</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="D236" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E236" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3"/>
+      <c r="C237" s="7"/>
+      <c r="D237" s="13"/>
+      <c r="E237" s="7"/>
+      <c r="F237" s="7"/>
+      <c r="G237" s="7"/>
+      <c r="H237" s="7"/>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>196</v>
-      </c>
-      <c r="C238" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D238" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E238" s="6" t="s">
-        <v>182</v>
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>225</v>
-      </c>
-      <c r="C239" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D239" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="E239" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F239" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B240" t="s">
-        <v>196</v>
-      </c>
-      <c r="C240" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D240" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E240" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="3"/>
-      <c r="C241" s="7"/>
-      <c r="D241" s="13"/>
-      <c r="E241" s="7"/>
-      <c r="F241" s="7"/>
-      <c r="G241" s="7"/>
-      <c r="H241" s="7"/>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B242" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B243" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>